<commit_message>
Upload Partial Result Done
</commit_message>
<xml_diff>
--- a/teacher/Grading_sheet.xlsx
+++ b/teacher/Grading_sheet.xlsx
@@ -51,7 +51,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="0" t="inlineStr">
         <is>
           <t>Seatno</t>
@@ -60,11 +60,6 @@
       <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Q1</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>Q2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Max Marks check
</commit_message>
<xml_diff>
--- a/teacher/Grading_sheet.xlsx
+++ b/teacher/Grading_sheet.xlsx
@@ -51,7 +51,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="0" t="inlineStr">
         <is>
           <t>Seatno</t>
@@ -60,6 +60,11 @@
       <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Q1</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Q2</t>
         </is>
       </c>
     </row>

</xml_diff>